<commit_message>
regex city + Order price per product count
</commit_message>
<xml_diff>
--- a/DW+P5+-+Modele+plan+tests+acceptation.xlsx
+++ b/DW+P5+-+Modele+plan+tests+acceptation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\P5-Dev-Web-Kanap-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC49F47-C8BA-41EB-AD5E-97CAAD6F43EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F520832-CB4E-4FBF-923F-9DF34F8F22D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="48">
   <si>
     <t>Fonctionnalité</t>
   </si>
@@ -146,6 +146,24 @@
   </si>
   <si>
     <t>Verifier chaque champ du formulaire.</t>
+  </si>
+  <si>
+    <t>Gestion des erreurs</t>
+  </si>
+  <si>
+    <t>Si erreur, afficher un message. Proposer d'envoyer un message au responsable du site.</t>
+  </si>
+  <si>
+    <t>Si aucune couleur specifié, afficher un message d'erreur pour la correction des champs.</t>
+  </si>
+  <si>
+    <t>Si la quantité specifié est hors limites, afficher un message d'erreur pour la correction des champs..</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Si un champ n'est pas valide, afficher un message d'erreur pour la correction des champs..</t>
   </si>
 </sst>
 </file>
@@ -772,10 +790,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -783,10 +801,10 @@
     <col min="1" max="1" width="7.28515625" customWidth="1"/>
     <col min="2" max="3" width="58.42578125" customWidth="1"/>
     <col min="4" max="4" width="57.85546875" customWidth="1"/>
-    <col min="5" max="5" width="52.7109375" customWidth="1"/>
+    <col min="5" max="6" width="52.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="30"/>
       <c r="B1" s="31" t="s">
         <v>0</v>
@@ -798,10 +816,13 @@
         <v>2</v>
       </c>
       <c r="E1" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="33" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="13" customFormat="1" ht="65.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" s="13" customFormat="1" ht="65.25" x14ac:dyDescent="0.2">
       <c r="A2" s="18">
         <v>1</v>
       </c>
@@ -815,10 +836,13 @@
         <v>6</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="13" customFormat="1" ht="43.5" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="13" customFormat="1" ht="43.5" x14ac:dyDescent="0.2">
       <c r="A3" s="22">
         <v>2</v>
       </c>
@@ -834,8 +858,11 @@
       <c r="E3" s="25" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" s="13" customFormat="1" ht="65.25" x14ac:dyDescent="0.2">
+      <c r="F3" s="25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="13" customFormat="1" ht="65.25" x14ac:dyDescent="0.2">
       <c r="A4" s="22">
         <v>3</v>
       </c>
@@ -849,10 +876,13 @@
         <v>13</v>
       </c>
       <c r="E4" s="25" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" s="13" customFormat="1" ht="65.25" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="13" customFormat="1" ht="65.25" x14ac:dyDescent="0.2">
       <c r="A5" s="22">
         <v>4</v>
       </c>
@@ -866,10 +896,13 @@
         <v>16</v>
       </c>
       <c r="E5" s="25" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="13" customFormat="1" ht="43.5" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+      <c r="F5" s="25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="13" customFormat="1" ht="65.25" x14ac:dyDescent="0.2">
       <c r="A6" s="22">
         <v>5</v>
       </c>
@@ -883,10 +916,13 @@
         <v>24</v>
       </c>
       <c r="E6" s="25" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="13" customFormat="1" ht="43.5" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+      <c r="F6" s="25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="13" customFormat="1" ht="65.25" x14ac:dyDescent="0.2">
       <c r="A7" s="14">
         <v>6</v>
       </c>
@@ -900,10 +936,13 @@
         <v>25</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" s="13" customFormat="1" ht="43.5" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="13" customFormat="1" ht="43.5" x14ac:dyDescent="0.2">
       <c r="A8" s="26">
         <v>7</v>
       </c>
@@ -917,10 +956,13 @@
         <v>20</v>
       </c>
       <c r="E8" s="29" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" s="13" customFormat="1" ht="65.25" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+      <c r="F8" s="29" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="13" customFormat="1" ht="65.25" x14ac:dyDescent="0.2">
       <c r="A9" s="14">
         <v>8</v>
       </c>
@@ -934,10 +976,13 @@
         <v>29</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" s="13" customFormat="1" ht="21.75" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="13" customFormat="1" ht="21.75" x14ac:dyDescent="0.2">
       <c r="A10" s="14">
         <v>9</v>
       </c>
@@ -950,11 +995,12 @@
       <c r="D10" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="17" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" s="13" customFormat="1" ht="43.5" x14ac:dyDescent="0.2">
+      <c r="E10" s="17"/>
+      <c r="F10" s="17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="13" customFormat="1" ht="65.25" x14ac:dyDescent="0.2">
       <c r="A11" s="14">
         <v>10</v>
       </c>
@@ -968,10 +1014,13 @@
         <v>35</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" s="13" customFormat="1" ht="65.25" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="13" customFormat="1" ht="65.25" x14ac:dyDescent="0.2">
       <c r="A12" s="14">
         <v>11</v>
       </c>
@@ -985,10 +1034,13 @@
         <v>33</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" s="13" customFormat="1" ht="43.5" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="13" customFormat="1" ht="65.25" x14ac:dyDescent="0.2">
       <c r="A13" s="14">
         <v>12</v>
       </c>
@@ -1002,10 +1054,13 @@
         <v>32</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" s="13" customFormat="1" ht="43.5" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="13" customFormat="1" ht="65.25" x14ac:dyDescent="0.2">
       <c r="A14" s="14">
         <v>13</v>
       </c>
@@ -1019,64 +1074,75 @@
         <v>34</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="21.75" x14ac:dyDescent="0.4">
+        <v>43</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="21.75" x14ac:dyDescent="0.4">
       <c r="A15" s="4"/>
       <c r="B15" s="1"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="3"/>
-    </row>
-    <row r="16" spans="1:5" ht="21.75" x14ac:dyDescent="0.4">
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="1:6" ht="21.75" x14ac:dyDescent="0.4">
       <c r="A16" s="4"/>
       <c r="B16" s="1"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="3"/>
-    </row>
-    <row r="17" spans="1:5" s="13" customFormat="1" ht="21.75" x14ac:dyDescent="0.2">
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" spans="1:6" s="13" customFormat="1" ht="21.75" x14ac:dyDescent="0.2">
       <c r="A17" s="11"/>
       <c r="B17" s="9"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="12"/>
-    </row>
-    <row r="18" spans="1:5" ht="21.75" x14ac:dyDescent="0.4">
+      <c r="F17" s="12"/>
+    </row>
+    <row r="18" spans="1:6" ht="21.75" x14ac:dyDescent="0.4">
       <c r="A18" s="4"/>
       <c r="B18" s="1"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="3"/>
-    </row>
-    <row r="19" spans="1:5" ht="21.75" x14ac:dyDescent="0.4">
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="1:6" ht="21.75" x14ac:dyDescent="0.4">
       <c r="A19" s="4"/>
       <c r="B19" s="1"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="3"/>
-    </row>
-    <row r="20" spans="1:5" ht="21.75" x14ac:dyDescent="0.4">
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" spans="1:6" ht="21.75" x14ac:dyDescent="0.4">
       <c r="A20" s="4"/>
       <c r="B20" s="1"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="3"/>
-    </row>
-    <row r="21" spans="1:5" ht="21.75" x14ac:dyDescent="0.4">
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="1:6" ht="21.75" x14ac:dyDescent="0.4">
       <c r="A21" s="4"/>
       <c r="B21" s="1"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="3"/>
-    </row>
-    <row r="22" spans="1:5" ht="21.75" x14ac:dyDescent="0.4">
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22" spans="1:6" ht="22.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A22" s="5"/>
       <c r="B22" s="6"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
       <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Gestion des erreurs, update du rapport.
</commit_message>
<xml_diff>
--- a/DW+P5+-+Modele+plan+tests+acceptation.xlsx
+++ b/DW+P5+-+Modele+plan+tests+acceptation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\P5-Dev-Web-Kanap-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F520832-CB4E-4FBF-923F-9DF34F8F22D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B564F4-DBCE-466F-80AC-66FE7E0059CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="53">
   <si>
     <t>Fonctionnalité</t>
   </si>
@@ -88,9 +88,6 @@
     <t>Edition du panier (nombre).</t>
   </si>
   <si>
-    <t xml:space="preserve"> Le cout total du panier est rafraichi.</t>
-  </si>
-  <si>
     <t>Création d'un local storage et ajout de l'article</t>
   </si>
   <si>
@@ -164,6 +161,25 @@
   </si>
   <si>
     <t>Si un champ n'est pas valide, afficher un message d'erreur pour la correction des champs..</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Le cout total du panier est rafraichi.
+La cout global de la ligne du produit est rafraichi.</t>
+  </si>
+  <si>
+    <t>Correction des champs du formulaire.</t>
+  </si>
+  <si>
+    <t>Si une erreur apparait sur un champ, la correction doit etre appliquée.</t>
+  </si>
+  <si>
+    <t>Les messages d'erreur de saisie doivent disparaitre.</t>
+  </si>
+  <si>
+    <t>Si le produit ne peut etre retrouvé, generer une exception.</t>
+  </si>
+  <si>
+    <t>Si le numero de commande n'est pas valide, afficher un message d'erreur pour la correction des champs..</t>
   </si>
 </sst>
 </file>
@@ -790,10 +806,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -816,7 +832,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F1" s="33" t="s">
         <v>3</v>
@@ -836,7 +852,7 @@
         <v>6</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F2" s="21" t="s">
         <v>7</v>
@@ -856,7 +872,7 @@
         <v>8</v>
       </c>
       <c r="E3" s="25" t="s">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="F3" s="25" t="s">
         <v>7</v>
@@ -876,7 +892,7 @@
         <v>13</v>
       </c>
       <c r="E4" s="25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F4" s="25" t="s">
         <v>7</v>
@@ -896,7 +912,7 @@
         <v>16</v>
       </c>
       <c r="E5" s="25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F5" s="25" t="s">
         <v>7</v>
@@ -910,13 +926,13 @@
         <v>17</v>
       </c>
       <c r="C6" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="24" t="s">
-        <v>24</v>
-      </c>
       <c r="E6" s="25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F6" s="25" t="s">
         <v>7</v>
@@ -933,10 +949,10 @@
         <v>19</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F7" s="17" t="s">
         <v>7</v>
@@ -947,16 +963,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="28" t="s">
         <v>26</v>
-      </c>
-      <c r="C8" s="28" t="s">
-        <v>27</v>
       </c>
       <c r="D8" s="28" t="s">
         <v>20</v>
       </c>
       <c r="E8" s="29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F8" s="29" t="s">
         <v>7</v>
@@ -967,22 +983,22 @@
         <v>8</v>
       </c>
       <c r="B9" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>29</v>
-      </c>
       <c r="E9" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F9" s="17" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="13" customFormat="1" ht="21.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" s="13" customFormat="1" ht="65.25" x14ac:dyDescent="0.2">
       <c r="A10" s="14">
         <v>9</v>
       </c>
@@ -990,10 +1006,10 @@
         <v>21</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="E10" s="17"/>
       <c r="F10" s="17" t="s">
@@ -1005,16 +1021,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F11" s="17" t="s">
         <v>7</v>
@@ -1025,16 +1041,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F12" s="17" t="s">
         <v>7</v>
@@ -1042,51 +1058,61 @@
     </row>
     <row r="13" spans="1:6" s="13" customFormat="1" ht="65.25" x14ac:dyDescent="0.2">
       <c r="A13" s="14">
+        <v>11</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="13" customFormat="1" ht="87" x14ac:dyDescent="0.2">
+      <c r="A14" s="14">
         <v>12</v>
       </c>
-      <c r="B13" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="16" t="s">
+      <c r="B14" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="F13" s="17" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" s="13" customFormat="1" ht="65.25" x14ac:dyDescent="0.2">
-      <c r="A14" s="14">
+      <c r="E14" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" s="13" customFormat="1" ht="43.5" x14ac:dyDescent="0.2">
+      <c r="A15" s="14">
         <v>13</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B15" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C15" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="E14" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="F14" s="17" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="21.75" x14ac:dyDescent="0.4">
-      <c r="A15" s="4"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
+      <c r="D15" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="16" spans="1:6" ht="21.75" x14ac:dyDescent="0.4">
       <c r="A16" s="4"/>
@@ -1096,21 +1122,21 @@
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:6" s="13" customFormat="1" ht="21.75" x14ac:dyDescent="0.2">
-      <c r="A17" s="11"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-    </row>
-    <row r="18" spans="1:6" ht="21.75" x14ac:dyDescent="0.4">
-      <c r="A18" s="4"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
+    <row r="17" spans="1:6" ht="21.75" x14ac:dyDescent="0.4">
+      <c r="A17" s="4"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="1:6" s="13" customFormat="1" ht="21.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="11"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
     </row>
     <row r="19" spans="1:6" ht="21.75" x14ac:dyDescent="0.4">
       <c r="A19" s="4"/>
@@ -1136,13 +1162,21 @@
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
     </row>
-    <row r="22" spans="1:6" ht="22.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="5"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
+    <row r="22" spans="1:6" ht="21.75" x14ac:dyDescent="0.4">
+      <c r="A22" s="4"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" spans="1:6" ht="22.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A23" s="5"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>